<commit_message>
Add initial bug report for product navigation issue (BUG_SORTED_002)
</commit_message>
<xml_diff>
--- a/02_test_cases/2_product_navigation/product_navigation.xlsx
+++ b/02_test_cases/2_product_navigation/product_navigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\swag_labs\swaglabs-qa-manual-project\02_test_cases\2_product_navigation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7C6375-222D-4813-9F5D-8A608474EE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881AEA5F-57D8-439A-AEE2-D95F876292CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE09C5C-271F-40FC-AAEF-2BAFE95B184D}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -637,7 +637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -660,7 +660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -683,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -706,7 +706,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -729,7 +729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -775,7 +775,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
@@ -798,7 +798,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>44</v>
       </c>
@@ -821,7 +821,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -844,7 +844,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>48</v>
       </c>

</xml_diff>